<commit_message>
Added p-values for the FMB and shanken correction t-stats.
</commit_message>
<xml_diff>
--- a/asset_pricing_analysis_report.xlsx
+++ b/asset_pricing_analysis_report.xlsx
@@ -1185,6 +1185,11 @@
           <t>t-Stat</t>
         </is>
       </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
     </row>
     <row r="59"/>
     <row r="60">
@@ -1202,6 +1207,9 @@
       <c r="D60" t="n">
         <v>3.888315326124474</v>
       </c>
+      <c r="E60" t="n">
+        <v>0.000119588677794491</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1218,6 +1226,9 @@
       <c r="D61" t="n">
         <v>-1.574614885272531</v>
       </c>
+      <c r="E61" t="n">
+        <v>0.1161976990350513</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1240,6 +1251,11 @@
       <c r="D66" t="inlineStr">
         <is>
           <t>t-Stat</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>p-value</t>
         </is>
       </c>
     </row>
@@ -1259,6 +1275,9 @@
       <c r="D68" t="n">
         <v>3.332377992672758</v>
       </c>
+      <c r="E68" t="n">
+        <v>0.0009476805940138444</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1275,6 +1294,9 @@
       <c r="D69" t="n">
         <v>-1.537806136582728</v>
       </c>
+      <c r="E69" t="n">
+        <v>0.1249484258211542</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1291,6 +1313,9 @@
       <c r="D70" t="n">
         <v>1.208829974844917</v>
       </c>
+      <c r="E70" t="n">
+        <v>0.2274980207316721</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1306,6 +1331,9 @@
       </c>
       <c r="D71" t="n">
         <v>3.958618582606134</v>
+      </c>
+      <c r="E71" t="n">
+        <v>9.036051523958477e-05</v>
       </c>
     </row>
   </sheetData>
@@ -1319,7 +1347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1343,21 +1371,48 @@
           <t>t-Stat</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
+          <t>Alpha</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.01560956353594066</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.004066792189690346</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3.838298788787928</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0001456096855874112</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
           <t>Beta_MKT</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B3" t="n">
         <v>-0.007206535691055282</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C3" t="n">
         <v>0.004636335842174735</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D3" t="n">
         <v>-1.554360153442845</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1209511400843071</v>
       </c>
     </row>
   </sheetData>
@@ -1371,7 +1426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1395,6 +1450,11 @@
           <t>t-Stat</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1411,6 +1471,9 @@
       <c r="D2" t="n">
         <v>3.332377992672758</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.0009476805940138444</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1427,6 +1490,9 @@
       <c r="D3" t="n">
         <v>-1.537806136582728</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.1249484258211542</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1443,6 +1509,9 @@
       <c r="D4" t="n">
         <v>1.208829974844917</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.2274980207316721</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1458,6 +1527,9 @@
       </c>
       <c r="D5" t="n">
         <v>3.958618582606134</v>
+      </c>
+      <c r="E5" t="n">
+        <v>9.036051523958477e-05</v>
       </c>
     </row>
   </sheetData>
@@ -1471,7 +1543,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1495,53 +1567,86 @@
           <t>t-Stat</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Beta_MKT</t>
+          <t>Alpha</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.006257984586878617</v>
+        <v>0.01129936010281002</v>
       </c>
       <c r="C2" t="n">
-        <v>0.004199246007045214</v>
+        <v>0.003498952205585338</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.490263865555719</v>
+        <v>3.229355372380616</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.001351352061958799</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Beta_SMB</t>
+          <t>Beta_MKT</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.001895011380758817</v>
+        <v>-0.006257984586878617</v>
       </c>
       <c r="C3" t="n">
-        <v>0.001617651707243008</v>
+        <v>0.004199246007045214</v>
       </c>
       <c r="D3" t="n">
-        <v>1.17145821456741</v>
+        <v>-1.490263865555719</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1370045312133752</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
+          <t>Beta_SMB</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.001895011380758817</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.001617651707243008</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.17145821456741</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.2421664339711995</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
           <t>Beta_HML</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B5" t="n">
         <v>0.005483763844750451</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" t="n">
         <v>0.001429464924243087</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" t="n">
         <v>3.836235329561617</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0001467905576828521</v>
       </c>
     </row>
   </sheetData>
@@ -8658,7 +8763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8682,6 +8787,11 @@
           <t>t-Stat</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>p-value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -8698,6 +8808,9 @@
       <c r="D2" t="n">
         <v>3.888315326124474</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.000119588677794491</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -8713,6 +8826,9 @@
       </c>
       <c r="D3" t="n">
         <v>-1.574614885272531</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1161976990350513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>